<commit_message>
aug update with ira revenues
</commit_message>
<xml_diff>
--- a/results/08-2022/comparison-deflators-08-2022.xlsx
+++ b/results/08-2022/comparison-deflators-08-2022.xlsx
@@ -760,25 +760,25 @@
         <v>-0.014</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.0522</v>
+        <v>-0.0703</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.0554</v>
+        <v>-0.0731</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.0378</v>
+        <v>-0.055</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.0318</v>
+        <v>-0.0487</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.0228</v>
+        <v>-0.0394</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.0112</v>
+        <v>-0.0275</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.0086</v>
+        <v>-0.0246</v>
       </c>
     </row>
     <row r="7">
@@ -872,13 +872,13 @@
         <v>-0.1373</v>
       </c>
       <c r="N8" t="n">
-        <v>0.1364</v>
+        <v>0.1478</v>
       </c>
       <c r="O8" t="n">
-        <v>0.1531</v>
+        <v>0.1643</v>
       </c>
       <c r="P8" t="n">
-        <v>0.2944</v>
+        <v>0.2998</v>
       </c>
     </row>
     <row r="9">
@@ -1207,28 +1207,28 @@
         <v>-3.3077</v>
       </c>
       <c r="I15" t="n">
-        <v>-2.0738</v>
+        <v>-2.0918</v>
       </c>
       <c r="J15" t="n">
-        <v>-2.0512</v>
+        <v>-2.087</v>
       </c>
       <c r="K15" t="n">
-        <v>-2.9627</v>
+        <v>-2.9915</v>
       </c>
       <c r="L15" t="n">
-        <v>-1.2317</v>
+        <v>-1.2599</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.9276</v>
+        <v>-0.9552</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.405</v>
+        <v>-0.4207</v>
       </c>
       <c r="O15" t="n">
-        <v>-0.5642</v>
+        <v>-0.5797</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.3977</v>
+        <v>-0.4185</v>
       </c>
     </row>
     <row r="16">
@@ -1557,28 +1557,28 @@
         <v>-0.0171</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.0121</v>
+        <v>-0.0172</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.0145</v>
+        <v>-0.0195</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.0157</v>
+        <v>-0.0206</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.0075</v>
+        <v>-0.0122</v>
       </c>
       <c r="M22" t="n">
-        <v>-0.0058</v>
+        <v>-0.0104</v>
       </c>
       <c r="N22" t="n">
-        <v>-0.0022</v>
+        <v>-0.0067</v>
       </c>
       <c r="O22" t="n">
-        <v>0.0007</v>
+        <v>-0.0037</v>
       </c>
       <c r="P22" t="n">
-        <v>0.0023</v>
+        <v>-0.002</v>
       </c>
     </row>
     <row r="23">
@@ -1657,28 +1657,28 @@
         <v>-0.1373</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.1289</v>
+        <v>-0.1418</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.0836</v>
+        <v>-0.0963</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.0609</v>
+        <v>-0.0672</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.0558</v>
+        <v>-0.062</v>
       </c>
       <c r="M24" t="n">
-        <v>-0.039</v>
+        <v>-0.0451</v>
       </c>
       <c r="N24" t="n">
-        <v>-0.0287</v>
+        <v>-0.0348</v>
       </c>
       <c r="O24" t="n">
-        <v>-0.0212</v>
+        <v>-0.0272</v>
       </c>
       <c r="P24" t="n">
-        <v>0.0051</v>
+        <v>-0.0009</v>
       </c>
     </row>
     <row r="25">
@@ -2110,25 +2110,25 @@
         <v>-0.0086</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.0087</v>
+        <v>-0.0268</v>
       </c>
       <c r="K33" t="n">
-        <v>-0.0088</v>
+        <v>-0.0265</v>
       </c>
       <c r="L33" t="n">
-        <v>-0.0089</v>
+        <v>-0.0262</v>
       </c>
       <c r="M33" t="n">
-        <v>-0.0089</v>
+        <v>-0.0258</v>
       </c>
       <c r="N33" t="n">
-        <v>-0.0088</v>
+        <v>-0.0254</v>
       </c>
       <c r="O33" t="n">
-        <v>-0.0087</v>
+        <v>-0.025</v>
       </c>
       <c r="P33" t="n">
-        <v>-0.0087</v>
+        <v>-0.0247</v>
       </c>
     </row>
     <row r="34">
@@ -2222,13 +2222,13 @@
         <v>-0.0075</v>
       </c>
       <c r="N35" t="n">
-        <v>-0.0077</v>
+        <v>0.0037</v>
       </c>
       <c r="O35" t="n">
-        <v>-0.0002</v>
+        <v>0.011</v>
       </c>
       <c r="P35" t="n">
-        <v>0.0001</v>
+        <v>0.0054</v>
       </c>
     </row>
     <row r="36">
@@ -2557,28 +2557,28 @@
         <v>0.2478</v>
       </c>
       <c r="I42" t="n">
-        <v>0.2274</v>
+        <v>0.2094</v>
       </c>
       <c r="J42" t="n">
-        <v>0.1434</v>
+        <v>0.1077</v>
       </c>
       <c r="K42" t="n">
-        <v>0.1013</v>
+        <v>0.0725</v>
       </c>
       <c r="L42" t="n">
-        <v>0.0543</v>
+        <v>0.0262</v>
       </c>
       <c r="M42" t="n">
-        <v>-0.0454</v>
+        <v>-0.073</v>
       </c>
       <c r="N42" t="n">
-        <v>-0.0426</v>
+        <v>-0.0583</v>
       </c>
       <c r="O42" t="n">
-        <v>-0.0341</v>
+        <v>-0.0495</v>
       </c>
       <c r="P42" t="n">
-        <v>-0.0287</v>
+        <v>-0.0496</v>
       </c>
     </row>
     <row r="43">
@@ -2907,28 +2907,28 @@
         <v>0.0015</v>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>-0.0052</v>
       </c>
       <c r="J49" t="n">
-        <v>0</v>
+        <v>-0.005</v>
       </c>
       <c r="K49" t="n">
-        <v>0</v>
+        <v>-0.0049</v>
       </c>
       <c r="L49" t="n">
-        <v>0</v>
+        <v>-0.0047</v>
       </c>
       <c r="M49" t="n">
-        <v>0</v>
+        <v>-0.0046</v>
       </c>
       <c r="N49" t="n">
-        <v>0</v>
+        <v>-0.0045</v>
       </c>
       <c r="O49" t="n">
-        <v>0</v>
+        <v>-0.0044</v>
       </c>
       <c r="P49" t="n">
-        <v>0</v>
+        <v>-0.0043</v>
       </c>
     </row>
     <row r="50">
@@ -3007,28 +3007,28 @@
         <v>-0.0101</v>
       </c>
       <c r="I51" t="n">
-        <v>0.0029</v>
+        <v>-0.01</v>
       </c>
       <c r="J51" t="n">
-        <v>0.0077</v>
+        <v>-0.005</v>
       </c>
       <c r="K51" t="n">
-        <v>0.0014</v>
+        <v>-0.0049</v>
       </c>
       <c r="L51" t="n">
-        <v>0.0014</v>
+        <v>-0.0048</v>
       </c>
       <c r="M51" t="n">
-        <v>0.0014</v>
+        <v>-0.0048</v>
       </c>
       <c r="N51" t="n">
-        <v>0.0013</v>
+        <v>-0.0047</v>
       </c>
       <c r="O51" t="n">
-        <v>0.0014</v>
+        <v>-0.0046</v>
       </c>
       <c r="P51" t="n">
-        <v>0.006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">

</xml_diff>